<commit_message>
clean up part 5
</commit_message>
<xml_diff>
--- a/input/Guedon1999_chemostat_data.xlsx
+++ b/input/Guedon1999_chemostat_data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idunmariaburgos/Documents/Work/Project/Ruminiclostridium cellulolyticum part 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Daniel/git/Ruminiclostridium-cellullolyticum-model-final/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F174CF1-E8A8-9141-B6D0-2FB4173049EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBCC240-89FA-3849-9B24-4445DC5F03D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{7C50BB4D-B114-A542-890D-3C33FA83E52C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7C50BB4D-B114-A542-890D-3C33FA83E52C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
   <si>
     <t>0.016</t>
   </si>
@@ -304,6 +305,33 @@
   </si>
   <si>
     <t>mu (growth rate)</t>
+  </si>
+  <si>
+    <t>Growth</t>
+  </si>
+  <si>
+    <t>R_EX_cellb_e</t>
+  </si>
+  <si>
+    <t>q_pyr</t>
+  </si>
+  <si>
+    <t>perc_ac</t>
+  </si>
+  <si>
+    <t>perc_lac</t>
+  </si>
+  <si>
+    <t>perc_etoh</t>
+  </si>
+  <si>
+    <t>R_EX_ac_e</t>
+  </si>
+  <si>
+    <t>R_EX_etoh_e</t>
+  </si>
+  <si>
+    <t>R_EX_lac__L_e</t>
   </si>
 </sst>
 </file>
@@ -370,11 +398,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E0A22E-94FA-3142-AF80-60259A0FBCF7}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="174" workbookViewId="0">
+      <selection activeCell="H6" sqref="B1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -862,4 +893,277 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9838543-4222-B642-9E95-E81A90B2D9D9}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="2" max="5" width="16.33203125" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4">
+        <f>$F2*G2/100</f>
+        <v>1.2192399999999999</v>
+      </c>
+      <c r="D2" s="4">
+        <f>$F2*H2/100</f>
+        <v>4.5639999999999993E-2</v>
+      </c>
+      <c r="E2" s="4">
+        <f>$F2*I2/100</f>
+        <v>0.36674999999999996</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:C8" si="0">$F3*G3/100</f>
+        <v>1.87005</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D8" si="1">$F3*H3/100</f>
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:E8" si="2">$F3*I3/100</f>
+        <v>0.80535000000000001</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
+        <v>1.86846</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="1"/>
+        <v>7.4499999999999997E-2</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="2"/>
+        <v>1.0400199999999999</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>2.09613</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.14445</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="2"/>
+        <v>0.98226000000000002</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>2.0996600000000001</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.25013999999999997</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="2"/>
+        <v>1.4402000000000001</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>2.1819699999999997</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.49104999999999999</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="2"/>
+        <v>1.6012499999999996</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>2.0792999999999999</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="1"/>
+        <v>0.36104999999999998</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="2"/>
+        <v>1.9096499999999998</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>